<commit_message>
filtrage recours par classe
</commit_message>
<xml_diff>
--- a/public/Deliberation database schema/deliberation.xlsx
+++ b/public/Deliberation database schema/deliberation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Deliberation database schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7474F8C-F2BB-4FEB-9358-8FADDAFEE2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BC9017-6739-4B54-8039-13D62F87B8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>semestre</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,6 +621,9 @@
       <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H10" s="2" t="s">
         <v>21</v>
       </c>
@@ -628,6 +631,11 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C12" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ajout des images en arrière plan
</commit_message>
<xml_diff>
--- a/public/Deliberation database schema/deliberation.xlsx
+++ b/public/Deliberation database schema/deliberation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Deliberation database schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BC9017-6739-4B54-8039-13D62F87B8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56F1FCF8-29AE-41A6-9BA7-99F49D0DC222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
         <v>27</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>

</xml_diff>